<commit_message>
Fix plots for easier visualization
</commit_message>
<xml_diff>
--- a/pythonForPlotting/i3g4250d_log.xlsx
+++ b/pythonForPlotting/i3g4250d_log.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\STM32F411\STM32F411_I3G4250D\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\STM32F411\STM32F411_I3G4250D\pythonForPlotting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{83700F84-2963-46B7-A9D4-B62D01E4F2D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A3DAC9B-D8B4-478B-AFF0-5BC2E836DEEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{DDD021AB-9AA3-403C-9FA6-3CDBC4D74C8B}"/>
   </bookViews>
@@ -41,1204 +41,1204 @@
     <t>i, rawRoll, filteredRoll</t>
   </si>
   <si>
-    <t>0,0.0026,0.0024</t>
-  </si>
-  <si>
-    <t>1,0.0047,0.0047</t>
-  </si>
-  <si>
-    <t>2,0.0056,0.0066</t>
-  </si>
-  <si>
-    <t>3,0.0049,0.0080</t>
-  </si>
-  <si>
-    <t>4,0.0031,0.0087</t>
-  </si>
-  <si>
-    <t>5,0.0010,0.0090</t>
-  </si>
-  <si>
-    <t>6,-0.0009,0.0089</t>
-  </si>
-  <si>
-    <t>7,-0.0026,0.0086</t>
-  </si>
-  <si>
-    <t>8,-0.0041,0.0080</t>
-  </si>
-  <si>
-    <t>9,-0.0051,0.0075</t>
-  </si>
-  <si>
-    <t>10,-0.0056,0.0070</t>
-  </si>
-  <si>
-    <t>11,-0.0058,0.0065</t>
-  </si>
-  <si>
-    <t>12,-0.0060,0.0061</t>
-  </si>
-  <si>
-    <t>13,-0.0063,0.0056</t>
-  </si>
-  <si>
-    <t>14,-0.0065,0.0053</t>
-  </si>
-  <si>
-    <t>15,-0.0068,0.0049</t>
-  </si>
-  <si>
-    <t>16,-0.0072,0.0045</t>
-  </si>
-  <si>
-    <t>17,-0.0079,0.0040</t>
-  </si>
-  <si>
-    <t>18,-0.0088,0.0034</t>
-  </si>
-  <si>
-    <t>19,-0.0097,0.0028</t>
-  </si>
-  <si>
-    <t>20,-0.0104,0.0022</t>
-  </si>
-  <si>
-    <t>21,-0.0105,0.0018</t>
-  </si>
-  <si>
-    <t>22,-0.0101,0.0015</t>
-  </si>
-  <si>
-    <t>23,-0.0094,0.0014</t>
-  </si>
-  <si>
-    <t>24,-0.0092,0.0012</t>
-  </si>
-  <si>
-    <t>25,-0.0094,0.0011</t>
-  </si>
-  <si>
-    <t>26,-0.0095,0.0010</t>
-  </si>
-  <si>
-    <t>27,-0.0095,0.0009</t>
-  </si>
-  <si>
-    <t>28,-0.0098,0.0007</t>
-  </si>
-  <si>
-    <t>29,-0.0110,0.0002</t>
-  </si>
-  <si>
-    <t>30,-0.0126,-0.0004</t>
-  </si>
-  <si>
-    <t>31,-0.0139,-0.0011</t>
-  </si>
-  <si>
-    <t>32,-0.0142,-0.0016</t>
-  </si>
-  <si>
-    <t>33,-0.0135,-0.0019</t>
-  </si>
-  <si>
-    <t>34,-0.0122,-0.0018</t>
-  </si>
-  <si>
-    <t>35,-0.0108,-0.0016</t>
-  </si>
-  <si>
-    <t>36,-0.0095,-0.0011</t>
-  </si>
-  <si>
-    <t>37,-0.0081,-0.0004</t>
-  </si>
-  <si>
-    <t>38,-0.0051,0.0009</t>
-  </si>
-  <si>
-    <t>39,0.0000,0.0030</t>
-  </si>
-  <si>
-    <t>40,0.0068,0.0060</t>
-  </si>
-  <si>
-    <t>41,0.0148,0.0100</t>
-  </si>
-  <si>
-    <t>42,0.0257,0.0157</t>
-  </si>
-  <si>
-    <t>43,0.0430,0.0242</t>
-  </si>
-  <si>
-    <t>44,0.0699,0.0368</t>
-  </si>
-  <si>
-    <t>45,0.1079,0.0547</t>
-  </si>
-  <si>
-    <t>46,0.1574,0.0792</t>
-  </si>
-  <si>
-    <t>47,0.2201,0.1114</t>
-  </si>
-  <si>
-    <t>48,0.2977,0.1527</t>
-  </si>
-  <si>
-    <t>49,0.3887,0.2034</t>
-  </si>
-  <si>
-    <t>50,0.4881,0.2628</t>
-  </si>
-  <si>
-    <t>51,0.5910,0.3299</t>
-  </si>
-  <si>
-    <t>52,0.6978,0.4044</t>
-  </si>
-  <si>
-    <t>53,0.8124,0.4868</t>
-  </si>
-  <si>
-    <t>54,0.9396,0.5782</t>
-  </si>
-  <si>
-    <t>55,1.0815,0.6795</t>
-  </si>
-  <si>
-    <t>56,1.2391,0.7920</t>
-  </si>
-  <si>
-    <t>57,1.4153,0.9174</t>
-  </si>
-  <si>
-    <t>58,1.6148,1.0577</t>
-  </si>
-  <si>
-    <t>59,1.8398,1.2146</t>
-  </si>
-  <si>
-    <t>60,2.0881,1.3890</t>
-  </si>
-  <si>
-    <t>61,2.3562,1.5810</t>
-  </si>
-  <si>
-    <t>62,2.6427,1.7909</t>
-  </si>
-  <si>
-    <t>63,2.9474,2.0185</t>
-  </si>
-  <si>
-    <t>64,3.2688,2.2636</t>
-  </si>
-  <si>
-    <t>65,3.6057,2.5259</t>
-  </si>
-  <si>
-    <t>66,3.9598,2.8056</t>
-  </si>
-  <si>
-    <t>67,4.3332,3.1031</t>
-  </si>
-  <si>
-    <t>68,4.7273,3.4190</t>
-  </si>
-  <si>
-    <t>69,5.1428,3.7539</t>
-  </si>
-  <si>
-    <t>70,5.5789,4.1077</t>
-  </si>
-  <si>
-    <t>71,6.0299,4.4787</t>
-  </si>
-  <si>
-    <t>72,6.4835,4.8632</t>
-  </si>
-  <si>
-    <t>73,6.9276,5.2567</t>
-  </si>
-  <si>
-    <t>74,7.3560,5.6549</t>
-  </si>
-  <si>
-    <t>75,7.7699,6.0549</t>
-  </si>
-  <si>
-    <t>76,8.1757,6.4556</t>
-  </si>
-  <si>
-    <t>77,8.5801,6.8572</t>
-  </si>
-  <si>
-    <t>78,8.9877,7.2602</t>
-  </si>
-  <si>
-    <t>79,9.3986,7.6646</t>
-  </si>
-  <si>
-    <t>80,9.8103,8.0702</t>
-  </si>
-  <si>
-    <t>81,10.2211,8.4766</t>
-  </si>
-  <si>
-    <t>82,10.6299,8.8832</t>
-  </si>
-  <si>
-    <t>83,11.0380,9.2903</t>
-  </si>
-  <si>
-    <t>84,11.4486,9.6983</t>
-  </si>
-  <si>
-    <t>85,11.8635,10.1078</t>
-  </si>
-  <si>
-    <t>86,12.2810,10.5185</t>
-  </si>
-  <si>
-    <t>87,12.6959,10.9295</t>
-  </si>
-  <si>
-    <t>88,13.1050,11.3398</t>
-  </si>
-  <si>
-    <t>89,13.5104,11.7492</t>
-  </si>
-  <si>
-    <t>90,13.9167,12.1584</t>
-  </si>
-  <si>
-    <t>91,14.3267,12.5680</t>
-  </si>
-  <si>
-    <t>92,14.7392,12.9780</t>
-  </si>
-  <si>
-    <t>93,15.1500,13.3878</t>
-  </si>
-  <si>
-    <t>94,15.5546,13.7957</t>
-  </si>
-  <si>
-    <t>95,15.9473,14.1997</t>
-  </si>
-  <si>
-    <t>96,16.3243,14.5977</t>
-  </si>
-  <si>
-    <t>97,16.6856,14.9882</t>
-  </si>
-  <si>
-    <t>98,17.0346,15.3708</t>
-  </si>
-  <si>
-    <t>99,17.3752,15.7457</t>
-  </si>
-  <si>
-    <t>100,17.7108,16.1137</t>
-  </si>
-  <si>
-    <t>101,18.0461,16.4764</t>
-  </si>
-  <si>
-    <t>102,18.3873,16.8362</t>
-  </si>
-  <si>
-    <t>103,18.7378,17.1953</t>
-  </si>
-  <si>
-    <t>104,19.0985,17.5556</t>
-  </si>
-  <si>
-    <t>105,19.4697,17.9185</t>
-  </si>
-  <si>
-    <t>106,19.8484,18.2843</t>
-  </si>
-  <si>
-    <t>107,20.2252,18.6509</t>
-  </si>
-  <si>
-    <t>108,20.5870,19.0147</t>
-  </si>
-  <si>
-    <t>109,20.9235,19.3712</t>
-  </si>
-  <si>
-    <t>110,21.2285,19.7159</t>
-  </si>
-  <si>
-    <t>111,21.4995,20.0452</t>
-  </si>
-  <si>
-    <t>112,21.7402,20.3572</t>
-  </si>
-  <si>
-    <t>113,21.9604,20.6525</t>
-  </si>
-  <si>
-    <t>114,22.1711,20.9329</t>
-  </si>
-  <si>
-    <t>115,22.3804,21.2014</t>
-  </si>
-  <si>
-    <t>116,22.5930,21.4607</t>
-  </si>
-  <si>
-    <t>117,22.8099,21.7128</t>
-  </si>
-  <si>
-    <t>118,23.0284,21.9592</t>
-  </si>
-  <si>
-    <t>119,23.2455,22.2002</t>
-  </si>
-  <si>
-    <t>120,23.4580,22.4356</t>
-  </si>
-  <si>
-    <t>121,23.6613,22.6644</t>
-  </si>
-  <si>
-    <t>122,23.8500,22.8848</t>
-  </si>
-  <si>
-    <t>123,24.0219,23.0956</t>
-  </si>
-  <si>
-    <t>124,24.1815,23.2972</t>
-  </si>
-  <si>
-    <t>125,24.3374,23.4911</t>
-  </si>
-  <si>
-    <t>126,24.4968,23.6796</t>
-  </si>
-  <si>
-    <t>127,24.6628,23.8647</t>
-  </si>
-  <si>
-    <t>128,24.8333,24.0474</t>
-  </si>
-  <si>
-    <t>129,25.0028,24.2273</t>
-  </si>
-  <si>
-    <t>130,25.1642,24.4029</t>
-  </si>
-  <si>
-    <t>131,25.3130,24.5729</t>
-  </si>
-  <si>
-    <t>132,25.4498,24.7364</t>
-  </si>
-  <si>
-    <t>133,25.5788,24.8935</t>
-  </si>
-  <si>
-    <t>134,25.7038,25.0449</t>
-  </si>
-  <si>
-    <t>135,25.8263,25.1912</t>
-  </si>
-  <si>
-    <t>136,25.9467,25.3328</t>
-  </si>
-  <si>
-    <t>137,26.0638,25.4697</t>
-  </si>
-  <si>
-    <t>138,26.1741,25.6012</t>
-  </si>
-  <si>
-    <t>139,26.2728,25.7258</t>
-  </si>
-  <si>
-    <t>140,26.3570,25.8422</t>
-  </si>
-  <si>
-    <t>141,26.4280,25.9500</t>
-  </si>
-  <si>
-    <t>142,26.4904,26.0495</t>
-  </si>
-  <si>
-    <t>143,26.5479,26.1414</t>
-  </si>
-  <si>
-    <t>144,26.6005,26.2260</t>
-  </si>
-  <si>
-    <t>145,26.6459,26.3031</t>
-  </si>
-  <si>
-    <t>146,26.6822,26.3724</t>
-  </si>
-  <si>
-    <t>147,26.7100,26.4339</t>
-  </si>
-  <si>
-    <t>148,26.7301,26.4876</t>
-  </si>
-  <si>
-    <t>149,26.7425,26.5336</t>
-  </si>
-  <si>
-    <t>150,26.7473,26.5718</t>
-  </si>
-  <si>
-    <t>151,26.7445,26.6023</t>
-  </si>
-  <si>
-    <t>152,26.7327,26.6246</t>
-  </si>
-  <si>
-    <t>153,26.7101,26.6381</t>
-  </si>
-  <si>
-    <t>154,26.6751,26.6423</t>
-  </si>
-  <si>
-    <t>155,26.6279,26.6366</t>
-  </si>
-  <si>
-    <t>156,26.5705,26.6214</t>
-  </si>
-  <si>
-    <t>157,26.5056,26.5972</t>
-  </si>
-  <si>
-    <t>158,26.4353,26.5646</t>
-  </si>
-  <si>
-    <t>159,26.3602,26.5243</t>
-  </si>
-  <si>
-    <t>160,26.2806,26.4768</t>
-  </si>
-  <si>
-    <t>161,26.1965,26.4227</t>
-  </si>
-  <si>
-    <t>162,26.1073,26.3620</t>
-  </si>
-  <si>
-    <t>163,26.0109,26.2943</t>
-  </si>
-  <si>
-    <t>164,25.9039,26.2187</t>
-  </si>
-  <si>
-    <t>165,25.7835,26.1343</t>
-  </si>
-  <si>
-    <t>166,25.6506,26.0407</t>
-  </si>
-  <si>
-    <t>167,25.5087,25.9383</t>
-  </si>
-  <si>
-    <t>168,25.3611,25.8276</t>
-  </si>
-  <si>
-    <t>169,25.2075,25.7089</t>
-  </si>
-  <si>
-    <t>170,25.0452,25.5818</t>
-  </si>
-  <si>
-    <t>171,24.8726,25.4460</t>
-  </si>
-  <si>
-    <t>172,24.6903,25.3014</t>
-  </si>
-  <si>
-    <t>173,24.4976,25.1474</t>
-  </si>
-  <si>
-    <t>174,24.2921,24.9834</t>
-  </si>
-  <si>
-    <t>175,24.0709,24.8081</t>
-  </si>
-  <si>
-    <t>176,23.8337,24.6209</t>
-  </si>
-  <si>
-    <t>177,23.5836,24.4222</t>
-  </si>
-  <si>
-    <t>178,23.3258,24.2130</t>
-  </si>
-  <si>
-    <t>179,23.0660,23.9953</t>
-  </si>
-  <si>
-    <t>180,22.8087,23.7711</t>
-  </si>
-  <si>
-    <t>181,22.5550,23.5420</t>
-  </si>
-  <si>
-    <t>182,22.3023,23.3086</t>
-  </si>
-  <si>
-    <t>183,22.0437,23.0698</t>
-  </si>
-  <si>
-    <t>184,21.7723,22.8241</t>
-  </si>
-  <si>
-    <t>185,21.4861,22.5704</t>
-  </si>
-  <si>
-    <t>186,21.1889,22.3087</t>
-  </si>
-  <si>
-    <t>187,20.8856,22.0396</t>
-  </si>
-  <si>
-    <t>188,20.5815,21.7647</t>
-  </si>
-  <si>
-    <t>189,20.2809,21.4859</t>
-  </si>
-  <si>
-    <t>190,19.9864,21.2048</t>
-  </si>
-  <si>
-    <t>191,19.6942,20.9215</t>
-  </si>
-  <si>
-    <t>192,19.3973,20.6352</t>
-  </si>
-  <si>
-    <t>193,19.0942,20.3458</t>
-  </si>
-  <si>
-    <t>194,18.7901,20.0544</t>
-  </si>
-  <si>
-    <t>195,18.4977,19.7655</t>
-  </si>
-  <si>
-    <t>196,18.2403,19.4858</t>
-  </si>
-  <si>
-    <t>197,18.0277,19.2207</t>
-  </si>
-  <si>
-    <t>198,17.8434,18.9697</t>
-  </si>
-  <si>
-    <t>199,17.6530,18.7267</t>
-  </si>
-  <si>
-    <t>200,17.4314,18.4846</t>
-  </si>
-  <si>
-    <t>201,17.1801,18.2390</t>
-  </si>
-  <si>
-    <t>202,16.9083,17.9877</t>
-  </si>
-  <si>
-    <t>203,16.6243,17.7301</t>
-  </si>
-  <si>
-    <t>204,16.3336,17.4664</t>
-  </si>
-  <si>
-    <t>205,16.0384,17.1968</t>
-  </si>
-  <si>
-    <t>206,15.7368,16.9209</t>
-  </si>
-  <si>
-    <t>207,15.4228,16.6369</t>
-  </si>
-  <si>
-    <t>208,15.0924,16.3439</t>
-  </si>
-  <si>
-    <t>209,14.7526,16.0431</t>
-  </si>
-  <si>
-    <t>210,14.4184,15.7378</t>
-  </si>
-  <si>
-    <t>211,14.1009,15.4320</t>
-  </si>
-  <si>
-    <t>212,13.7997,15.1277</t>
-  </si>
-  <si>
-    <t>213,13.5059,14.8255</t>
-  </si>
-  <si>
-    <t>214,13.2122,14.5244</t>
-  </si>
-  <si>
-    <t>215,12.9154,14.2238</t>
-  </si>
-  <si>
-    <t>216,12.6149,13.9229</t>
-  </si>
-  <si>
-    <t>217,12.3119,13.6216</t>
-  </si>
-  <si>
-    <t>218,12.0097,13.3205</t>
-  </si>
-  <si>
-    <t>219,11.7114,13.0203</t>
-  </si>
-  <si>
-    <t>220,11.4184,12.7216</t>
-  </si>
-  <si>
-    <t>221,11.1286,12.4246</t>
-  </si>
-  <si>
-    <t>222,10.8383,12.1284</t>
-  </si>
-  <si>
-    <t>223,10.5434,11.8319</t>
-  </si>
-  <si>
-    <t>224,10.2418,11.5339</t>
-  </si>
-  <si>
-    <t>225,9.9344,11.2340</t>
-  </si>
-  <si>
-    <t>226,9.6249,10.9327</t>
-  </si>
-  <si>
-    <t>227,9.3189,10.6312</t>
-  </si>
-  <si>
-    <t>228,9.0225,10.3317</t>
-  </si>
-  <si>
-    <t>229,8.7390,10.0361</t>
-  </si>
-  <si>
-    <t>230,8.4676,9.7453</t>
-  </si>
-  <si>
-    <t>231,8.2030,9.4592</t>
-  </si>
-  <si>
-    <t>232,7.9380,9.1762</t>
-  </si>
-  <si>
-    <t>233,7.6657,8.8941</t>
-  </si>
-  <si>
-    <t>234,7.3815,8.6105</t>
-  </si>
-  <si>
-    <t>235,7.0840,8.3234</t>
-  </si>
-  <si>
-    <t>236,6.7753,8.0320</t>
-  </si>
-  <si>
-    <t>237,6.4614,7.7369</t>
-  </si>
-  <si>
-    <t>238,6.1522,7.4405</t>
-  </si>
-  <si>
-    <t>239,5.8580,7.1463</t>
-  </si>
-  <si>
-    <t>240,5.5869,6.8583</t>
-  </si>
-  <si>
-    <t>241,5.3416,6.5797</t>
-  </si>
-  <si>
-    <t>242,5.1189,6.3122</t>
-  </si>
-  <si>
-    <t>243,4.9128,6.0563</t>
-  </si>
-  <si>
-    <t>244,4.7173,5.8115</t>
-  </si>
-  <si>
-    <t>245,4.5289,5.5769</t>
-  </si>
-  <si>
-    <t>246,4.3472,5.3520</t>
-  </si>
-  <si>
-    <t>247,4.1735,5.1368</t>
-  </si>
-  <si>
-    <t>248,4.0098,4.9312</t>
-  </si>
-  <si>
-    <t>249,3.8557,4.7352</t>
-  </si>
-  <si>
-    <t>250,3.7088,4.5481</t>
-  </si>
-  <si>
-    <t>251,3.5666,4.3690</t>
-  </si>
-  <si>
-    <t>252,3.4282,4.1973</t>
-  </si>
-  <si>
-    <t>253,3.2964,4.0334</t>
-  </si>
-  <si>
-    <t>254,3.1766,3.8785</t>
-  </si>
-  <si>
-    <t>255,3.0734,3.7339</t>
-  </si>
-  <si>
-    <t>256,2.9866,3.6004</t>
-  </si>
-  <si>
-    <t>257,2.9118,3.4776</t>
-  </si>
-  <si>
-    <t>258,2.8444,3.3648</t>
-  </si>
-  <si>
-    <t>259,2.7814,3.2609</t>
-  </si>
-  <si>
-    <t>260,2.7217,3.1648</t>
-  </si>
-  <si>
-    <t>261,2.6650,3.0757</t>
-  </si>
-  <si>
-    <t>262,2.6118,2.9932</t>
-  </si>
-  <si>
-    <t>263,2.5632,2.9169</t>
-  </si>
-  <si>
-    <t>264,2.5193,2.8466</t>
-  </si>
-  <si>
-    <t>265,2.4801,2.7821</t>
-  </si>
-  <si>
-    <t>266,2.4471,2.7237</t>
-  </si>
-  <si>
-    <t>267,2.4233,2.6722</t>
-  </si>
-  <si>
-    <t>268,2.4100,2.6280</t>
-  </si>
-  <si>
-    <t>269,2.4040,2.5907</t>
-  </si>
-  <si>
-    <t>270,2.4002,2.5590</t>
-  </si>
-  <si>
-    <t>271,2.3956,2.5320</t>
-  </si>
-  <si>
-    <t>272,2.3904,2.5086</t>
-  </si>
-  <si>
-    <t>273,2.3848,2.4883</t>
-  </si>
-  <si>
-    <t>274,2.3793,2.4707</t>
-  </si>
-  <si>
-    <t>275,2.3769,2.4564</t>
-  </si>
-  <si>
-    <t>276,2.3831,2.4466</t>
-  </si>
-  <si>
-    <t>277,2.4012,2.4425</t>
-  </si>
-  <si>
-    <t>278,2.4297,2.4448</t>
-  </si>
-  <si>
-    <t>279,2.4676,2.4542</t>
-  </si>
-  <si>
-    <t>280,2.5178,2.4720</t>
-  </si>
-  <si>
-    <t>281,2.5858,2.5001</t>
-  </si>
-  <si>
-    <t>282,2.6737,2.5402</t>
-  </si>
-  <si>
-    <t>283,2.7798,2.5929</t>
-  </si>
-  <si>
-    <t>284,2.9001,2.6583</t>
-  </si>
-  <si>
-    <t>285,3.0337,2.7368</t>
-  </si>
-  <si>
-    <t>286,3.1850,2.8298</t>
-  </si>
-  <si>
-    <t>287,3.3611,2.9396</t>
-  </si>
-  <si>
-    <t>288,3.5681,3.0690</t>
-  </si>
-  <si>
-    <t>289,3.8078,3.2200</t>
-  </si>
-  <si>
-    <t>290,4.0779,3.3938</t>
-  </si>
-  <si>
-    <t>291,4.3744,3.5906</t>
-  </si>
-  <si>
-    <t>292,4.6928,3.8100</t>
-  </si>
-  <si>
-    <t>293,5.0294,4.0508</t>
-  </si>
-  <si>
-    <t>294,5.3804,4.3117</t>
-  </si>
-  <si>
-    <t>295,5.7439,4.5912</t>
-  </si>
-  <si>
-    <t>296,6.1209,4.8889</t>
-  </si>
-  <si>
-    <t>297,6.5135,5.2042</t>
-  </si>
-  <si>
-    <t>298,6.9210,5.5363</t>
-  </si>
-  <si>
-    <t>299,7.3387,5.8837</t>
-  </si>
-  <si>
-    <t>300,7.7610,6.2440</t>
-  </si>
-  <si>
-    <t>301,8.1839,6.6150</t>
-  </si>
-  <si>
-    <t>302,8.6060,6.9948</t>
-  </si>
-  <si>
-    <t>303,9.0277,7.3817</t>
-  </si>
-  <si>
-    <t>304,9.4500,7.7749</t>
-  </si>
-  <si>
-    <t>305,9.8733,8.1733</t>
-  </si>
-  <si>
-    <t>306,10.2975,8.5761</t>
-  </si>
-  <si>
-    <t>307,10.7216,8.9825</t>
-  </si>
-  <si>
-    <t>308,11.1445,9.3916</t>
-  </si>
-  <si>
-    <t>309,11.5652,9.8024</t>
-  </si>
-  <si>
-    <t>310,11.9839,10.2146</t>
-  </si>
-  <si>
-    <t>311,12.4027,10.6281</t>
-  </si>
-  <si>
-    <t>312,12.8244,11.0433</t>
-  </si>
-  <si>
-    <t>313,13.2489,11.4601</t>
-  </si>
-  <si>
-    <t>314,13.6725,11.8777</t>
-  </si>
-  <si>
-    <t>315,14.0889,12.2940</t>
-  </si>
-  <si>
-    <t>316,14.4925,12.7068</t>
-  </si>
-  <si>
-    <t>317,14.8814,13.1143</t>
-  </si>
-  <si>
-    <t>318,15.2566,13.5154</t>
-  </si>
-  <si>
-    <t>319,15.6222,13.9098</t>
-  </si>
-  <si>
-    <t>320,15.9827,14.2982</t>
-  </si>
-  <si>
-    <t>321,16.3414,14.6814</t>
-  </si>
-  <si>
-    <t>322,16.6995,15.0603</t>
-  </si>
-  <si>
-    <t>323,17.0570,15.4356</t>
-  </si>
-  <si>
-    <t>324,17.4169,15.8088</t>
-  </si>
-  <si>
-    <t>325,17.7846,16.1820</t>
-  </si>
-  <si>
-    <t>326,18.1640,16.5572</t>
-  </si>
-  <si>
-    <t>327,18.5526,16.9351</t>
-  </si>
-  <si>
-    <t>328,18.9438,17.3151</t>
-  </si>
-  <si>
-    <t>329,19.3311,17.6956</t>
-  </si>
-  <si>
-    <t>330,19.7077,18.0741</t>
-  </si>
-  <si>
-    <t>331,20.0677,18.4478</t>
-  </si>
-  <si>
-    <t>332,20.4105,18.8152</t>
-  </si>
-  <si>
-    <t>333,20.7439,19.1766</t>
-  </si>
-  <si>
-    <t>334,21.0776,19.5336</t>
-  </si>
-  <si>
-    <t>335,21.4137,19.8868</t>
-  </si>
-  <si>
-    <t>336,21.7471,20.2361</t>
-  </si>
-  <si>
-    <t>337,22.0727,20.5805</t>
-  </si>
-  <si>
-    <t>338,22.3898,20.9195</t>
-  </si>
-  <si>
-    <t>339,22.6989,21.2527</t>
-  </si>
-  <si>
-    <t>340,22.9996,21.5795</t>
-  </si>
-  <si>
-    <t>341,23.2899,21.8990</t>
-  </si>
-  <si>
-    <t>342,23.5679,22.2102</t>
-  </si>
-  <si>
-    <t>343,23.8319,22.5121</t>
-  </si>
-  <si>
-    <t>344,24.0820,22.8039</t>
-  </si>
-  <si>
-    <t>345,24.3190,23.0852</t>
-  </si>
-  <si>
-    <t>346,24.5443,23.3561</t>
-  </si>
-  <si>
-    <t>347,24.7597,23.6167</t>
-  </si>
-  <si>
-    <t>348,24.9671,23.8676</t>
-  </si>
-  <si>
-    <t>349,25.1696,24.1100</t>
-  </si>
-  <si>
-    <t>350,25.3707,24.3455</t>
-  </si>
-  <si>
-    <t>351,25.5737,24.5756</t>
-  </si>
-  <si>
-    <t>352,25.7785,24.8012</t>
-  </si>
-  <si>
-    <t>353,25.9810,25.0223</t>
-  </si>
-  <si>
-    <t>354,26.1757,25.2378</t>
-  </si>
-  <si>
-    <t>355,26.3564,25.4458</t>
-  </si>
-  <si>
-    <t>356,26.5182,25.6440</t>
-  </si>
-  <si>
-    <t>357,26.6587,25.8306</t>
-  </si>
-  <si>
-    <t>358,26.7798,26.0045</t>
-  </si>
-  <si>
-    <t>359,26.8853,26.1654</t>
-  </si>
-  <si>
-    <t>360,26.9768,26.3132</t>
-  </si>
-  <si>
-    <t>361,27.0532,26.4473</t>
-  </si>
-  <si>
-    <t>362,27.1133,26.5673</t>
-  </si>
-  <si>
-    <t>363,27.1587,26.6736</t>
-  </si>
-  <si>
-    <t>364,27.1947,26.7675</t>
-  </si>
-  <si>
-    <t>365,27.2283,26.8512</t>
-  </si>
-  <si>
-    <t>366,27.2654,26.9274</t>
-  </si>
-  <si>
-    <t>367,27.3086,26.9984</t>
-  </si>
-  <si>
-    <t>368,27.3561,27.0654</t>
-  </si>
-  <si>
-    <t>369,27.4033,27.1287</t>
-  </si>
-  <si>
-    <t>370,27.4449,27.1875</t>
-  </si>
-  <si>
-    <t>371,27.4769,27.2406</t>
-  </si>
-  <si>
-    <t>372,27.4962,27.2867</t>
-  </si>
-  <si>
-    <t>373,27.4998,27.3239</t>
-  </si>
-  <si>
-    <t>374,27.4858,27.3509</t>
-  </si>
-  <si>
-    <t>375,27.4542,27.3663</t>
-  </si>
-  <si>
-    <t>376,27.4071,27.3699</t>
-  </si>
-  <si>
-    <t>377,27.3481,27.3620</t>
-  </si>
-  <si>
-    <t>378,27.2812,27.3435</t>
-  </si>
-  <si>
-    <t>379,27.2107,27.3160</t>
-  </si>
-  <si>
-    <t>380,27.1389,27.2808</t>
-  </si>
-  <si>
-    <t>381,27.0660,27.2390</t>
-  </si>
-  <si>
-    <t>382,26.9906,27.1910</t>
-  </si>
-  <si>
-    <t>383,26.9102,27.1368</t>
-  </si>
-  <si>
-    <t>384,26.8217,27.0759</t>
-  </si>
-  <si>
-    <t>385,26.7222,27.0073</t>
-  </si>
-  <si>
-    <t>386,26.6109,26.9303</t>
-  </si>
-  <si>
-    <t>387,26.4874,26.8443</t>
-  </si>
-  <si>
-    <t>388,26.3524,26.7490</t>
-  </si>
-  <si>
-    <t>389,26.2081,26.6447</t>
-  </si>
-  <si>
-    <t>390,26.0575,26.5320</t>
-  </si>
-  <si>
-    <t>391,25.9022,26.4117</t>
-  </si>
-  <si>
-    <t>392,25.7424,26.2841</t>
-  </si>
-  <si>
-    <t>393,25.5786,26.1501</t>
-  </si>
-  <si>
-    <t>394,25.4120,26.0102</t>
-  </si>
-  <si>
-    <t>395,25.2415,25.8645</t>
-  </si>
-  <si>
-    <t>396,25.0631,25.7122</t>
-  </si>
-  <si>
-    <t>397,24.8725,25.5521</t>
-  </si>
-  <si>
-    <t>398,24.6681,25.3832</t>
-  </si>
-  <si>
-    <t>399,24.4494,25.2044</t>
+    <t>0,-0.0029,-0.0011</t>
+  </si>
+  <si>
+    <t>1,-0.0049,-0.0020</t>
+  </si>
+  <si>
+    <t>2,-0.0041,-0.0023</t>
+  </si>
+  <si>
+    <t>3,-0.0066,-0.0035</t>
+  </si>
+  <si>
+    <t>4,-0.0071,-0.0038</t>
+  </si>
+  <si>
+    <t>5,-0.0061,-0.0031</t>
+  </si>
+  <si>
+    <t>6,-0.0056,-0.0034</t>
+  </si>
+  <si>
+    <t>7,-0.0082,-0.0040</t>
+  </si>
+  <si>
+    <t>8,-0.0071,-0.0039</t>
+  </si>
+  <si>
+    <t>9,-0.0056,-0.0042</t>
+  </si>
+  <si>
+    <t>10,-0.0082,-0.0046</t>
+  </si>
+  <si>
+    <t>11,-0.0092,-0.0052</t>
+  </si>
+  <si>
+    <t>12,-0.0104,-0.0065</t>
+  </si>
+  <si>
+    <t>13,-0.0124,-0.0081</t>
+  </si>
+  <si>
+    <t>14,-0.0151,-0.0100</t>
+  </si>
+  <si>
+    <t>15,-0.0158,-0.0107</t>
+  </si>
+  <si>
+    <t>16,-0.0155,-0.0111</t>
+  </si>
+  <si>
+    <t>17,-0.0147,-0.0105</t>
+  </si>
+  <si>
+    <t>18,-0.0141,-0.0098</t>
+  </si>
+  <si>
+    <t>19,-0.0135,-0.0090</t>
+  </si>
+  <si>
+    <t>20,-0.0136,-0.0083</t>
+  </si>
+  <si>
+    <t>21,-0.0114,-0.0077</t>
+  </si>
+  <si>
+    <t>22,-0.0116,-0.0080</t>
+  </si>
+  <si>
+    <t>23,-0.0116,-0.0083</t>
+  </si>
+  <si>
+    <t>24,-0.0116,-0.0087</t>
+  </si>
+  <si>
+    <t>25,-0.0124,-0.0085</t>
+  </si>
+  <si>
+    <t>26,-0.0131,-0.0083</t>
+  </si>
+  <si>
+    <t>27,-0.0144,-0.0089</t>
+  </si>
+  <si>
+    <t>28,-0.0151,-0.0095</t>
+  </si>
+  <si>
+    <t>29,-0.0158,-0.0099</t>
+  </si>
+  <si>
+    <t>30,-0.0148,-0.0095</t>
+  </si>
+  <si>
+    <t>31,-0.0123,-0.0084</t>
+  </si>
+  <si>
+    <t>32,-0.0098,-0.0066</t>
+  </si>
+  <si>
+    <t>33,-0.0071,-0.0051</t>
+  </si>
+  <si>
+    <t>34,-0.0057,-0.0035</t>
+  </si>
+  <si>
+    <t>35,-0.0057,-0.0020</t>
+  </si>
+  <si>
+    <t>36,-0.0044,-0.0005</t>
+  </si>
+  <si>
+    <t>37,-0.0054,-0.0000</t>
+  </si>
+  <si>
+    <t>38,-0.0052,0.0006</t>
+  </si>
+  <si>
+    <t>39,-0.0019,0.0027</t>
+  </si>
+  <si>
+    <t>40,0.0046,0.0066</t>
+  </si>
+  <si>
+    <t>41,0.0119,0.0127</t>
+  </si>
+  <si>
+    <t>42,0.0257,0.0212</t>
+  </si>
+  <si>
+    <t>43,0.0401,0.0314</t>
+  </si>
+  <si>
+    <t>44,0.0556,0.0433</t>
+  </si>
+  <si>
+    <t>45,0.0732,0.0589</t>
+  </si>
+  <si>
+    <t>46,0.1065,0.0929</t>
+  </si>
+  <si>
+    <t>47,0.2291,0.1676</t>
+  </si>
+  <si>
+    <t>48,0.4257,0.2872</t>
+  </si>
+  <si>
+    <t>49,0.6552,0.4470</t>
+  </si>
+  <si>
+    <t>50,0.9297,0.6530</t>
+  </si>
+  <si>
+    <t>51,1.2759,0.9168</t>
+  </si>
+  <si>
+    <t>52,1.7158,1.2541</t>
+  </si>
+  <si>
+    <t>53,2.2827,1.6849</t>
+  </si>
+  <si>
+    <t>54,2.9757,2.2121</t>
+  </si>
+  <si>
+    <t>55,3.7493,2.8268</t>
+  </si>
+  <si>
+    <t>56,4.5822,3.5185</t>
+  </si>
+  <si>
+    <t>57,5.4662,4.2788</t>
+  </si>
+  <si>
+    <t>58,6.4023,5.0996</t>
+  </si>
+  <si>
+    <t>59,7.3575,5.9566</t>
+  </si>
+  <si>
+    <t>60,8.2660,6.8181</t>
+  </si>
+  <si>
+    <t>61,9.0884,7.6474</t>
+  </si>
+  <si>
+    <t>62,9.7720,8.4060</t>
+  </si>
+  <si>
+    <t>63,10.2775,9.0484</t>
+  </si>
+  <si>
+    <t>64,10.5507,9.5347</t>
+  </si>
+  <si>
+    <t>65,10.5633,9.8368</t>
+  </si>
+  <si>
+    <t>66,10.3726,9.9554</t>
+  </si>
+  <si>
+    <t>67,10.0009,9.8936</t>
+  </si>
+  <si>
+    <t>68,9.4801,9.6718</t>
+  </si>
+  <si>
+    <t>69,8.8671,9.3157</t>
+  </si>
+  <si>
+    <t>70,8.1841,8.8481</t>
+  </si>
+  <si>
+    <t>71,7.4422,8.2829</t>
+  </si>
+  <si>
+    <t>72,6.6256,7.6278</t>
+  </si>
+  <si>
+    <t>73,5.7420,6.8909</t>
+  </si>
+  <si>
+    <t>74,4.7950,6.0767</t>
+  </si>
+  <si>
+    <t>75,3.7774,5.1900</t>
+  </si>
+  <si>
+    <t>76,2.7102,4.2404</t>
+  </si>
+  <si>
+    <t>77,1.6071,3.2392</t>
+  </si>
+  <si>
+    <t>78,0.4877,2.2324</t>
+  </si>
+  <si>
+    <t>79,-0.0090,1.4321</t>
+  </si>
+  <si>
+    <t>80,-0.4608,0.7290</t>
+  </si>
+  <si>
+    <t>81,-0.9630,0.0890</t>
+  </si>
+  <si>
+    <t>82,-1.3639,-0.4412</t>
+  </si>
+  <si>
+    <t>83,-1.5625,-0.8447</t>
+  </si>
+  <si>
+    <t>84,-1.6333,-1.1282</t>
+  </si>
+  <si>
+    <t>85,-1.6040,-1.2981</t>
+  </si>
+  <si>
+    <t>86,-1.4807,-1.3611</t>
+  </si>
+  <si>
+    <t>87,-1.2650,-1.3197</t>
+  </si>
+  <si>
+    <t>88,-0.9381,-1.1704</t>
+  </si>
+  <si>
+    <t>89,-0.4996,-0.9138</t>
+  </si>
+  <si>
+    <t>90,0.0475,-0.5810</t>
+  </si>
+  <si>
+    <t>91,0.2790,-0.2738</t>
+  </si>
+  <si>
+    <t>92,0.6089,0.0773</t>
+  </si>
+  <si>
+    <t>93,1.1466,0.4985</t>
+  </si>
+  <si>
+    <t>94,1.7228,0.9680</t>
+  </si>
+  <si>
+    <t>95,2.3109,1.4824</t>
+  </si>
+  <si>
+    <t>96,2.9474,2.0407</t>
+  </si>
+  <si>
+    <t>97,3.6175,2.6372</t>
+  </si>
+  <si>
+    <t>98,4.3029,3.2613</t>
+  </si>
+  <si>
+    <t>99,4.9794,3.8971</t>
+  </si>
+  <si>
+    <t>100,5.6175,4.5238</t>
+  </si>
+  <si>
+    <t>101,6.1885,5.1189</t>
+  </si>
+  <si>
+    <t>102,6.6610,5.6558</t>
+  </si>
+  <si>
+    <t>103,7.0056,6.1105</t>
+  </si>
+  <si>
+    <t>104,7.2077,6.4627</t>
+  </si>
+  <si>
+    <t>105,7.2671,6.7005</t>
+  </si>
+  <si>
+    <t>106,7.1860,6.8158</t>
+  </si>
+  <si>
+    <t>107,6.9652,6.8030</t>
+  </si>
+  <si>
+    <t>108,6.6054,6.6659</t>
+  </si>
+  <si>
+    <t>109,6.1440,6.4134</t>
+  </si>
+  <si>
+    <t>110,5.5897,6.0495</t>
+  </si>
+  <si>
+    <t>111,4.9328,5.5795</t>
+  </si>
+  <si>
+    <t>112,4.1888,5.0130</t>
+  </si>
+  <si>
+    <t>113,3.3867,4.3667</t>
+  </si>
+  <si>
+    <t>114,2.5529,3.6564</t>
+  </si>
+  <si>
+    <t>115,1.6886,2.8937</t>
+  </si>
+  <si>
+    <t>116,0.8012,2.0888</t>
+  </si>
+  <si>
+    <t>117,0.0846,1.4418</t>
+  </si>
+  <si>
+    <t>118,-0.1859,0.9028</t>
+  </si>
+  <si>
+    <t>119,-0.5926,0.3824</t>
+  </si>
+  <si>
+    <t>120,-1.0452,-0.0929</t>
+  </si>
+  <si>
+    <t>121,-1.3465,-0.4965</t>
+  </si>
+  <si>
+    <t>122,-1.5470,-0.8226</t>
+  </si>
+  <si>
+    <t>123,-1.6555,-1.0643</t>
+  </si>
+  <si>
+    <t>124,-1.6594,-1.2147</t>
+  </si>
+  <si>
+    <t>125,-1.5490,-1.2636</t>
+  </si>
+  <si>
+    <t>126,-1.3178,-1.2065</t>
+  </si>
+  <si>
+    <t>127,-0.9681,-1.0391</t>
+  </si>
+  <si>
+    <t>128,-0.5045,-0.7610</t>
+  </si>
+  <si>
+    <t>129,0.0696,-0.4364</t>
+  </si>
+  <si>
+    <t>130,0.2732,-0.1415</t>
+  </si>
+  <si>
+    <t>131,0.5824,0.1983</t>
+  </si>
+  <si>
+    <t>132,1.1043,0.6027</t>
+  </si>
+  <si>
+    <t>133,1.6410,1.0465</t>
+  </si>
+  <si>
+    <t>134,2.1831,1.5287</t>
+  </si>
+  <si>
+    <t>135,2.7695,2.0488</t>
+  </si>
+  <si>
+    <t>136,3.3830,2.5970</t>
+  </si>
+  <si>
+    <t>137,3.9836,3.1575</t>
+  </si>
+  <si>
+    <t>138,4.5505,3.7099</t>
+  </si>
+  <si>
+    <t>139,5.0448,4.2284</t>
+  </si>
+  <si>
+    <t>140,5.4346,4.6878</t>
+  </si>
+  <si>
+    <t>141,5.6991,5.0627</t>
+  </si>
+  <si>
+    <t>142,5.8161,5.3332</t>
+  </si>
+  <si>
+    <t>143,5.7878,5.4865</t>
+  </si>
+  <si>
+    <t>144,5.6153,5.5168</t>
+  </si>
+  <si>
+    <t>145,5.3181,5.4257</t>
+  </si>
+  <si>
+    <t>146,4.9031,5.2151</t>
+  </si>
+  <si>
+    <t>147,4.3750,4.8878</t>
+  </si>
+  <si>
+    <t>148,3.7428,4.4495</t>
+  </si>
+  <si>
+    <t>149,3.0161,3.9065</t>
+  </si>
+  <si>
+    <t>150,2.2026,3.2672</t>
+  </si>
+  <si>
+    <t>151,1.3159,2.5407</t>
+  </si>
+  <si>
+    <t>152,0.3725,1.7802</t>
+  </si>
+  <si>
+    <t>153,-0.0088,1.1455</t>
+  </si>
+  <si>
+    <t>154,-0.4061,0.5553</t>
+  </si>
+  <si>
+    <t>155,-0.9748,-0.0159</t>
+  </si>
+  <si>
+    <t>156,-1.4172,-0.5216</t>
+  </si>
+  <si>
+    <t>157,-1.7290,-0.9538</t>
+  </si>
+  <si>
+    <t>158,-1.9544,-1.3044</t>
+  </si>
+  <si>
+    <t>159,-2.0650,-1.5613</t>
+  </si>
+  <si>
+    <t>160,-2.0630,-1.7187</t>
+  </si>
+  <si>
+    <t>161,-1.9495,-1.7738</t>
+  </si>
+  <si>
+    <t>162,-1.7246,-1.7233</t>
+  </si>
+  <si>
+    <t>163,-1.3889,-1.5651</t>
+  </si>
+  <si>
+    <t>164,-0.9393,-1.2965</t>
+  </si>
+  <si>
+    <t>165,-0.3710,-0.9162</t>
+  </si>
+  <si>
+    <t>166,0.2559,-0.5537</t>
+  </si>
+  <si>
+    <t>167,0.5107,-0.2122</t>
+  </si>
+  <si>
+    <t>168,0.9336,0.1906</t>
+  </si>
+  <si>
+    <t>169,1.5053,0.6409</t>
+  </si>
+  <si>
+    <t>170,2.0486,1.1221</t>
+  </si>
+  <si>
+    <t>171,2.6166,1.6377</t>
+  </si>
+  <si>
+    <t>172,3.2217,2.1815</t>
+  </si>
+  <si>
+    <t>173,3.8218,2.7365</t>
+  </si>
+  <si>
+    <t>174,4.3690,3.2762</t>
+  </si>
+  <si>
+    <t>175,4.8268,3.7736</t>
+  </si>
+  <si>
+    <t>176,5.1733,4.2050</t>
+  </si>
+  <si>
+    <t>177,5.3964,4.5502</t>
+  </si>
+  <si>
+    <t>178,5.4843,4.7919</t>
+  </si>
+  <si>
+    <t>179,5.4260,4.9152</t>
+  </si>
+  <si>
+    <t>180,5.2121,4.9091</t>
+  </si>
+  <si>
+    <t>181,4.8494,4.7679</t>
+  </si>
+  <si>
+    <t>182,4.3426,4.4890</t>
+  </si>
+  <si>
+    <t>183,3.6887,4.0712</t>
+  </si>
+  <si>
+    <t>184,2.9054,3.5217</t>
+  </si>
+  <si>
+    <t>185,2.0219,2.8549</t>
+  </si>
+  <si>
+    <t>186,1.0662,2.0868</t>
+  </si>
+  <si>
+    <t>187,0.1879,1.4297</t>
+  </si>
+  <si>
+    <t>188,-0.2438,0.8218</t>
+  </si>
+  <si>
+    <t>189,-0.8410,0.1952</t>
+  </si>
+  <si>
+    <t>190,-1.4465,-0.3943</t>
+  </si>
+  <si>
+    <t>191,-1.8765,-0.9153</t>
+  </si>
+  <si>
+    <t>192,-2.1992,-1.3563</t>
+  </si>
+  <si>
+    <t>193,-2.3966,-1.6982</t>
+  </si>
+  <si>
+    <t>194,-2.4453,-1.9240</t>
+  </si>
+  <si>
+    <t>195,-2.3407,-2.0240</t>
+  </si>
+  <si>
+    <t>196,-2.0939,-1.9937</t>
+  </si>
+  <si>
+    <t>197,-1.7109,-1.8304</t>
+  </si>
+  <si>
+    <t>198,-1.1874,-1.5322</t>
+  </si>
+  <si>
+    <t>199,-0.5306,-1.1014</t>
+  </si>
+  <si>
+    <t>200,0.2340,-0.6522</t>
+  </si>
+  <si>
+    <t>201,0.6229,-0.2111</t>
+  </si>
+  <si>
+    <t>202,1.1630,0.2951</t>
+  </si>
+  <si>
+    <t>203,1.8530,0.8560</t>
+  </si>
+  <si>
+    <t>204,2.5166,1.4482</t>
+  </si>
+  <si>
+    <t>205,3.1767,2.0605</t>
+  </si>
+  <si>
+    <t>206,3.8163,2.6727</t>
+  </si>
+  <si>
+    <t>207,4.3796,3.2512</t>
+  </si>
+  <si>
+    <t>208,4.8228,3.7640</t>
+  </si>
+  <si>
+    <t>209,5.1140,4.1813</t>
+  </si>
+  <si>
+    <t>210,5.2402,4.4806</t>
+  </si>
+  <si>
+    <t>211,5.1931,4.6449</t>
+  </si>
+  <si>
+    <t>212,4.9785,4.6656</t>
+  </si>
+  <si>
+    <t>213,4.6118,4.5434</t>
+  </si>
+  <si>
+    <t>214,4.1144,4.2853</t>
+  </si>
+  <si>
+    <t>215,3.5029,3.8979</t>
+  </si>
+  <si>
+    <t>216,2.7789,3.3871</t>
+  </si>
+  <si>
+    <t>217,1.9447,2.7601</t>
+  </si>
+  <si>
+    <t>218,1.0265,2.0301</t>
+  </si>
+  <si>
+    <t>219,0.2045,1.3958</t>
+  </si>
+  <si>
+    <t>220,-0.3154,0.7735</t>
+  </si>
+  <si>
+    <t>221,-0.9754,0.1284</t>
+  </si>
+  <si>
+    <t>222,-1.5951,-0.4831</t>
+  </si>
+  <si>
+    <t>223,-2.0647,-1.0316</t>
+  </si>
+  <si>
+    <t>224,-2.4139,-1.4977</t>
+  </si>
+  <si>
+    <t>225,-2.6334,-1.8635</t>
+  </si>
+  <si>
+    <t>226,-2.7039,-2.1118</t>
+  </si>
+  <si>
+    <t>227,-2.6130,-2.2283</t>
+  </si>
+  <si>
+    <t>228,-2.3629,-2.2061</t>
+  </si>
+  <si>
+    <t>229,-1.9649,-2.0419</t>
+  </si>
+  <si>
+    <t>230,-1.4159,-1.7344</t>
+  </si>
+  <si>
+    <t>231,-0.7249,-1.2874</t>
+  </si>
+  <si>
+    <t>232,0.0870,-0.7567</t>
+  </si>
+  <si>
+    <t>233,0.5609,-0.2040</t>
+  </si>
+  <si>
+    <t>234,1.2018,0.3972</t>
+  </si>
+  <si>
+    <t>235,1.9430,1.0403</t>
+  </si>
+  <si>
+    <t>236,2.6642,1.7050</t>
+  </si>
+  <si>
+    <t>237,3.3608,2.3734</t>
+  </si>
+  <si>
+    <t>238,4.0000,3.0180</t>
+  </si>
+  <si>
+    <t>239,4.5352,3.6072</t>
+  </si>
+  <si>
+    <t>240,4.9317,4.1093</t>
+  </si>
+  <si>
+    <t>241,5.1512,4.4915</t>
+  </si>
+  <si>
+    <t>242,5.1729,4.7299</t>
+  </si>
+  <si>
+    <t>243,5.0032,4.8117</t>
+  </si>
+  <si>
+    <t>244,4.6595,4.7366</t>
+  </si>
+  <si>
+    <t>245,4.1720,4.5112</t>
+  </si>
+  <si>
+    <t>246,3.5555,4.1450</t>
+  </si>
+  <si>
+    <t>247,2.8291,3.6520</t>
+  </si>
+  <si>
+    <t>248,2.0140,3.0446</t>
+  </si>
+  <si>
+    <t>249,1.1194,2.3366</t>
+  </si>
+  <si>
+    <t>250,0.1870,1.6792</t>
+  </si>
+  <si>
+    <t>251,-0.3022,1.0078</t>
+  </si>
+  <si>
+    <t>252,-0.9981,0.3491</t>
+  </si>
+  <si>
+    <t>253,-1.5894,-0.2718</t>
+  </si>
+  <si>
+    <t>254,-2.0631,-0.8250</t>
+  </si>
+  <si>
+    <t>255,-2.3960,-1.2865</t>
+  </si>
+  <si>
+    <t>256,-2.5911,-1.6421</t>
+  </si>
+  <si>
+    <t>257,-2.6372,-1.8738</t>
+  </si>
+  <si>
+    <t>258,-2.5209,-1.9718</t>
+  </si>
+  <si>
+    <t>259,-2.2525,-1.9323</t>
+  </si>
+  <si>
+    <t>260,-1.8473,-1.7551</t>
+  </si>
+  <si>
+    <t>261,-1.2946,-1.4396</t>
+  </si>
+  <si>
+    <t>262,-0.6165,-0.9925</t>
+  </si>
+  <si>
+    <t>263,0.1626,-0.5183</t>
+  </si>
+  <si>
+    <t>264,0.7180,0.0188</t>
+  </si>
+  <si>
+    <t>265,1.3953,0.5983</t>
+  </si>
+  <si>
+    <t>266,2.0410,1.1856</t>
+  </si>
+  <si>
+    <t>267,2.6102,1.7551</t>
+  </si>
+  <si>
+    <t>268,3.0953,2.2824</t>
+  </si>
+  <si>
+    <t>269,3.4711,2.7406</t>
+  </si>
+  <si>
+    <t>270,3.7048,3.1038</t>
+  </si>
+  <si>
+    <t>271,3.7786,3.3484</t>
+  </si>
+  <si>
+    <t>272,3.6764,3.4585</t>
+  </si>
+  <si>
+    <t>273,3.4181,3.4304</t>
+  </si>
+  <si>
+    <t>274,3.0220,3.2679</t>
+  </si>
+  <si>
+    <t>275,2.5151,2.9826</t>
+  </si>
+  <si>
+    <t>276,1.9175,2.5854</t>
+  </si>
+  <si>
+    <t>277,1.2375,2.0881</t>
+  </si>
+  <si>
+    <t>278,0.4891,1.5283</t>
+  </si>
+  <si>
+    <t>279,0.1236,0.9946</t>
+  </si>
+  <si>
+    <t>280,-0.5023,0.4449</t>
+  </si>
+  <si>
+    <t>281,-1.0483,-0.0921</t>
+  </si>
+  <si>
+    <t>282,-1.5138,-0.5954</t>
+  </si>
+  <si>
+    <t>283,-1.8978,-1.0466</t>
+  </si>
+  <si>
+    <t>284,-2.1809,-1.4258</t>
+  </si>
+  <si>
+    <t>285,-2.3383,-1.7132</t>
+  </si>
+  <si>
+    <t>286,-2.3508,-1.8905</t>
+  </si>
+  <si>
+    <t>287,-2.2135,-1.9453</t>
+  </si>
+  <si>
+    <t>288,-1.9235,-1.8690</t>
+  </si>
+  <si>
+    <t>289,-1.4917,-1.6602</t>
+  </si>
+  <si>
+    <t>290,-0.9329,-1.3245</t>
+  </si>
+  <si>
+    <t>291,-0.2725,-0.8722</t>
+  </si>
+  <si>
+    <t>292,0.3800,-0.4391</t>
+  </si>
+  <si>
+    <t>293,0.9744,0.0450</t>
+  </si>
+  <si>
+    <t>294,1.5531,0.5548</t>
+  </si>
+  <si>
+    <t>295,2.0953,1.0664</t>
+  </si>
+  <si>
+    <t>296,2.5734,1.5539</t>
+  </si>
+  <si>
+    <t>297,2.9568,1.9893</t>
+  </si>
+  <si>
+    <t>298,3.2050,2.3412</t>
+  </si>
+  <si>
+    <t>299,3.2900,2.5799</t>
+  </si>
+  <si>
+    <t>300,3.1897,2.6830</t>
+  </si>
+  <si>
+    <t>301,2.9064,2.6386</t>
+  </si>
+  <si>
+    <t>302,2.4589,2.4434</t>
+  </si>
+  <si>
+    <t>303,1.8636,2.1030</t>
+  </si>
+  <si>
+    <t>304,1.1497,1.6294</t>
+  </si>
+  <si>
+    <t>305,0.3653,1.1602</t>
+  </si>
+  <si>
+    <t>306,-0.0673,0.6239</t>
+  </si>
+  <si>
+    <t>307,-0.8045,0.0549</t>
+  </si>
+  <si>
+    <t>308,-1.4249,-0.5243</t>
+  </si>
+  <si>
+    <t>309,-1.9882,-1.0863</t>
+  </si>
+  <si>
+    <t>310,-2.4695,-1.6073</t>
+  </si>
+  <si>
+    <t>311,-2.8467,-2.0653</t>
+  </si>
+  <si>
+    <t>312,-3.0993,-2.4370</t>
+  </si>
+  <si>
+    <t>313,-3.2086,-2.7018</t>
+  </si>
+  <si>
+    <t>314,-3.1634,-2.8445</t>
+  </si>
+  <si>
+    <t>315,-2.9619,-2.8567</t>
+  </si>
+  <si>
+    <t>316,-2.6164,-2.7345</t>
+  </si>
+  <si>
+    <t>317,-2.1354,-2.4807</t>
+  </si>
+  <si>
+    <t>318,-1.5349,-2.1011</t>
+  </si>
+  <si>
+    <t>319,-0.8347,-1.6087</t>
+  </si>
+  <si>
+    <t>320,-0.0627,-1.0244</t>
+  </si>
+  <si>
+    <t>321,0.4610,-0.4608</t>
+  </si>
+  <si>
+    <t>322,1.0646,0.0912</t>
+  </si>
+  <si>
+    <t>323,1.5421,0.5987</t>
+  </si>
+  <si>
+    <t>324,1.8867,1.0304</t>
+  </si>
+  <si>
+    <t>325,2.0693,1.3577</t>
+  </si>
+  <si>
+    <t>326,2.0810,1.5554</t>
+  </si>
+  <si>
+    <t>327,1.8979,1.6030</t>
+  </si>
+  <si>
+    <t>328,1.5221,1.4882</t>
+  </si>
+  <si>
+    <t>329,0.9738,1.2139</t>
+  </si>
+  <si>
+    <t>330,0.3120,0.9036</t>
+  </si>
+  <si>
+    <t>331,-0.0154,0.5212</t>
+  </si>
+  <si>
+    <t>332,-0.6751,0.0679</t>
+  </si>
+  <si>
+    <t>333,-1.2414,-0.4187</t>
+  </si>
+  <si>
+    <t>334,-1.7735,-0.9077</t>
+  </si>
+  <si>
+    <t>335,-2.2281,-1.3728</t>
+  </si>
+  <si>
+    <t>336,-2.5901,-1.7883</t>
+  </si>
+  <si>
+    <t>337,-2.8358,-2.1284</t>
+  </si>
+  <si>
+    <t>338,-2.9397,-2.3709</t>
+  </si>
+  <si>
+    <t>339,-2.8984,-2.5006</t>
+  </si>
+  <si>
+    <t>340,-2.7083,-2.5082</t>
+  </si>
+  <si>
+    <t>341,-2.3792,-2.3903</t>
+  </si>
+  <si>
+    <t>342,-1.9273,-2.1502</t>
+  </si>
+  <si>
+    <t>343,-1.3673,-1.7950</t>
+  </si>
+  <si>
+    <t>344,-0.7139,-1.3344</t>
+  </si>
+  <si>
+    <t>345,0.0116,-0.7944</t>
+  </si>
+  <si>
+    <t>346,0.4370,-0.2466</t>
+  </si>
+  <si>
+    <t>347,1.0279,0.3045</t>
+  </si>
+  <si>
+    <t>348,1.5553,0.8369</t>
+  </si>
+  <si>
+    <t>349,2.0034,1.3259</t>
+  </si>
+  <si>
+    <t>350,2.3342,1.7440</t>
+  </si>
+  <si>
+    <t>351,2.5224,2.0626</t>
+  </si>
+  <si>
+    <t>352,2.5270,2.2524</t>
+  </si>
+  <si>
+    <t>353,2.3341,2.2896</t>
+  </si>
+  <si>
+    <t>354,1.9422,2.1627</t>
+  </si>
+  <si>
+    <t>355,1.3700,1.8700</t>
+  </si>
+  <si>
+    <t>356,0.6437,1.4248</t>
+  </si>
+  <si>
+    <t>357,0.1374,0.9863</t>
+  </si>
+  <si>
+    <t>358,-0.5542,0.4265</t>
+  </si>
+  <si>
+    <t>359,-1.2952,-0.1736</t>
+  </si>
+  <si>
+    <t>360,-1.9738,-0.7885</t>
+  </si>
+  <si>
+    <t>361,-2.5808,-1.3879</t>
+  </si>
+  <si>
+    <t>362,-3.0964,-1.9426</t>
+  </si>
+  <si>
+    <t>363,-3.4901,-2.4247</t>
+  </si>
+  <si>
+    <t>364,-3.7393,-2.8105</t>
+  </si>
+  <si>
+    <t>365,-3.8376,-3.0802</t>
+  </si>
+  <si>
+    <t>366,-3.7781,-3.2222</t>
+  </si>
+  <si>
+    <t>367,-3.5637,-3.2273</t>
+  </si>
+  <si>
+    <t>368,-3.1960,-3.0929</t>
+  </si>
+  <si>
+    <t>369,-2.6830,-2.8190</t>
+  </si>
+  <si>
+    <t>370,-2.0459,-2.4128</t>
+  </si>
+  <si>
+    <t>371,-1.3004,-1.8877</t>
+  </si>
+  <si>
+    <t>372,-0.4862,-1.2661</t>
+  </si>
+  <si>
+    <t>373,0.3240,-0.6810</t>
+  </si>
+  <si>
+    <t>374,0.9684,-0.0888</t>
+  </si>
+  <si>
+    <t>375,1.5189,0.4715</t>
+  </si>
+  <si>
+    <t>376,1.9494,0.9711</t>
+  </si>
+  <si>
+    <t>377,2.2470,1.3847</t>
+  </si>
+  <si>
+    <t>378,2.3971,1.6902</t>
+  </si>
+  <si>
+    <t>379,2.3844,1.8696</t>
+  </si>
+  <si>
+    <t>380,2.2030,1.9086</t>
+  </si>
+  <si>
+    <t>381,1.8512,1.8012</t>
+  </si>
+  <si>
+    <t>382,1.3492,1.5495</t>
+  </si>
+  <si>
+    <t>383,0.7186,1.1662</t>
+  </si>
+  <si>
+    <t>384,0.3038,0.7714</t>
+  </si>
+  <si>
+    <t>385,-0.3320,0.3044</t>
+  </si>
+  <si>
+    <t>386,-0.9098,-0.1964</t>
+  </si>
+  <si>
+    <t>387,-1.4537,-0.7023</t>
+  </si>
+  <si>
+    <t>388,-1.9459,-1.1935</t>
+  </si>
+  <si>
+    <t>389,-2.3682,-1.6499</t>
+  </si>
+  <si>
+    <t>390,-2.7004,-2.0503</t>
+  </si>
+  <si>
+    <t>391,-2.9166,-2.3731</t>
+  </si>
+  <si>
+    <t>392,-3.0046,-2.6006</t>
+  </si>
+  <si>
+    <t>393,-2.9522,-2.7181</t>
+  </si>
+  <si>
+    <t>394,-2.7629,-2.7186</t>
+  </si>
+  <si>
+    <t>395,-2.4454,-2.6014</t>
+  </si>
+  <si>
+    <t>396,-2.0155,-2.3713</t>
+  </si>
+  <si>
+    <t>397,-1.4976,-2.0394</t>
+  </si>
+  <si>
+    <t>398,-0.9154,-1.6217</t>
+  </si>
+  <si>
+    <t>399,-0.2898,-1.1339</t>
   </si>
 </sst>
 </file>
@@ -1612,7 +1612,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F99B0AE-DCE7-4985-A49C-3490E8B97651}">
   <dimension ref="A1:A401"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>

</xml_diff>